<commit_message>
updated features, squashed ai crash, squashed text bug
</commit_message>
<xml_diff>
--- a/Features.xlsx
+++ b/Features.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\jarre\Documents\university\Digipen\2020Fall\CS529\JTEFinal\JTE_FinalProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University\Digipen\CS529\CS529_FinalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9523B502-C25B-4068-A33C-B3AE47890D66}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D7B35D7-A172-4363-9186-61D4B70077E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{85BFBB5D-1747-4A29-9807-EDEF17AFBFDA}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{85BFBB5D-1747-4A29-9807-EDEF17AFBFDA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="61">
   <si>
     <t>Feature Name</t>
   </si>
@@ -135,9 +134,6 @@
     <t>deemed unnecessary</t>
   </si>
   <si>
-    <t>Work in progress</t>
-  </si>
-  <si>
     <t>main.cpp</t>
   </si>
   <si>
@@ -193,6 +189,33 @@
   </si>
   <si>
     <t>PhysicsManager.h, PhysicsBody.h, Events.h</t>
+  </si>
+  <si>
+    <t>Sort-of</t>
+  </si>
+  <si>
+    <t>GraphicsManager</t>
+  </si>
+  <si>
+    <t>I have four render layers. Not using any depth buffer as that was unnecessary, but this does do some sorting.</t>
+  </si>
+  <si>
+    <t>Ingame: Pause menu-&gt;Debug-&gt;Toggle Collision Drawing</t>
+  </si>
+  <si>
+    <t>Most collisions will be 'piercing', though this can be modified in config.json</t>
+  </si>
+  <si>
+    <t>AIEnemyCore, AIEnemyStationary, AIEnemyChase, AIMissile</t>
+  </si>
+  <si>
+    <t>Can be clunky for earlier components built while I was still learning.</t>
+  </si>
+  <si>
+    <t>Turret, AIMissile, ControllerShip, Events.h, FollowCursor, TargetLock</t>
+  </si>
+  <si>
+    <t>Press 'T' to target an enemy, then press space to launch a missile at them.</t>
   </si>
 </sst>
 </file>
@@ -335,19 +358,19 @@
       </border>
     </dxf>
     <dxf>
+      <border outline="0">
+        <bottom style="thick">
+          <color theme="4"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor rgb="FFA5A5A5"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thick">
-          <color theme="4"/>
-        </bottom>
-      </border>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -363,7 +386,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FD1E5249-7267-474A-8393-D322FE22626B}" name="Table2" displayName="Table2" ref="A1:D1048576" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="3" headerRowCellStyle="Heading 1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FD1E5249-7267-474A-8393-D322FE22626B}" name="Table2" displayName="Table2" ref="A1:D1048576" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="2" headerRowCellStyle="Heading 1">
   <autoFilter ref="A1:D1048576" xr:uid="{09CCFD5E-A0B5-41B7-B9A6-8644BC4455D8}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{A33BE97F-2568-4269-91CF-DD54C10EC3A6}" name="Feature Name"/>
@@ -672,10 +695,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AC5A136-341D-4CE6-A487-D300FB9FAEEA}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -708,7 +731,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -719,7 +742,7 @@
         <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -730,7 +753,7 @@
         <v>30</v>
       </c>
       <c r="C4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -741,7 +764,7 @@
         <v>30</v>
       </c>
       <c r="C5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -752,7 +775,7 @@
         <v>30</v>
       </c>
       <c r="C6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -763,7 +786,7 @@
         <v>30</v>
       </c>
       <c r="C7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -774,7 +797,10 @@
         <v>30</v>
       </c>
       <c r="C8" t="s">
-        <v>40</v>
+        <v>39</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -785,7 +811,7 @@
         <v>30</v>
       </c>
       <c r="C9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -796,7 +822,7 @@
         <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -807,7 +833,7 @@
         <v>30</v>
       </c>
       <c r="C11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -818,7 +844,7 @@
         <v>30</v>
       </c>
       <c r="C12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -826,10 +852,13 @@
         <v>14</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>33</v>
+        <v>4</v>
       </c>
       <c r="C13" t="s">
-        <v>45</v>
+        <v>44</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -840,7 +869,7 @@
         <v>30</v>
       </c>
       <c r="C14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -851,7 +880,7 @@
         <v>30</v>
       </c>
       <c r="C15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -862,10 +891,10 @@
         <v>30</v>
       </c>
       <c r="C16" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -873,10 +902,10 @@
         <v>30</v>
       </c>
       <c r="C17" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -884,27 +913,27 @@
         <v>31</v>
       </c>
       <c r="C18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>21</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="C19" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -912,10 +941,10 @@
         <v>30</v>
       </c>
       <c r="C20" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -923,10 +952,10 @@
         <v>30</v>
       </c>
       <c r="C21" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -934,37 +963,49 @@
         <v>30</v>
       </c>
       <c r="C22" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>25</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>33</v>
+        <v>4</v>
       </c>
       <c r="C23" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>26</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="C24" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>27</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="C25" t="s">
+        <v>59</v>
+      </c>
+      <c r="F25" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
controls and tutorial done
</commit_message>
<xml_diff>
--- a/Features.xlsx
+++ b/Features.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University\Digipen\CS529\CS529_FinalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D7B35D7-A172-4363-9186-61D4B70077E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4091B57-47C4-4C8A-A79F-38A145190AA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{85BFBB5D-1747-4A29-9807-EDEF17AFBFDA}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="62">
   <si>
     <t>Feature Name</t>
   </si>
@@ -216,6 +216,9 @@
   </si>
   <si>
     <t>Press 'T' to target an enemy, then press space to launch a missile at them.</t>
+  </si>
+  <si>
+    <t>GameStateManager, Resources Menus, Resource Level archetypes Menus. Accessible ingame via main menu and pause menu.</t>
   </si>
 </sst>
 </file>
@@ -697,8 +700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AC5A136-341D-4CE6-A487-D300FB9FAEEA}">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1010,7 +1013,10 @@
         <v>28</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>31</v>
+        <v>4</v>
+      </c>
+      <c r="C26" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>